<commit_message>
Corrected obj val and added diff
</commit_message>
<xml_diff>
--- a/main/results/CIRED/FinalValuesCIREDResults.xlsx
+++ b/main/results/CIRED/FinalValuesCIREDResults.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paugm\OneDrive\Documentos\Universitat\CITCEA\agistin\main\results\CIRED\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergi Costa\Documents\agistin\main\results\CIRED\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A6DEE9D-0466-4936-9288-F83E607A9F05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07ED3C66-6481-4553-B31C-7561A5E25212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{868BAA8E-1AA2-4D5F-B31E-70B0642F7C3D}"/>
+    <workbookView xWindow="4740" yWindow="2520" windowWidth="19755" windowHeight="12510" xr2:uid="{868BAA8E-1AA2-4D5F-B31E-70B0642F7C3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Wmin</t>
   </si>
@@ -49,15 +47,32 @@
   <si>
     <t>Month</t>
   </si>
+  <si>
+    <t>PV diff</t>
+  </si>
+  <si>
+    <t>Obj corr</t>
+  </si>
+  <si>
+    <t>Diff</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="#,##0.0000"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,15 +98,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -107,7 +130,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -403,18 +426,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95B29B87-BC7A-4D90-BE76-F4D7E2AFE4B5}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.1796875" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -427,8 +450,17 @@
       <c r="D1" t="s">
         <v>1</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>8500</v>
       </c>
@@ -441,8 +473,23 @@
       <c r="D2">
         <v>9500</v>
       </c>
+      <c r="E2" s="2">
+        <v>0.40994366040178998</v>
+      </c>
+      <c r="F2" s="3">
+        <f>C2-E2</f>
+        <v>19.420056339598208</v>
+      </c>
+      <c r="G2" s="5">
+        <f>(F2-$F$2)</f>
+        <v>0</v>
+      </c>
+      <c r="H2" s="4">
+        <f>G2/$F$2</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>8500</v>
       </c>
@@ -455,8 +502,16 @@
       <c r="D3">
         <v>10500</v>
       </c>
+      <c r="E3" s="2">
+        <v>0.37253296342661602</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" ref="F3:F7" si="0">C3-E3</f>
+        <v>-3.2963426616017255E-5</v>
+      </c>
+      <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>9000</v>
       </c>
@@ -467,10 +522,25 @@
         <v>19.2</v>
       </c>
       <c r="D4">
-        <v>9050</v>
+        <v>9500</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.40994369703737998</v>
+      </c>
+      <c r="F4" s="3">
+        <f t="shared" si="0"/>
+        <v>18.790056302962618</v>
+      </c>
+      <c r="G4" s="7">
+        <f>(F4-$F$2)</f>
+        <v>-0.63000003663558957</v>
+      </c>
+      <c r="H4" s="4">
+        <f>G4/$F$2</f>
+        <v>-3.2440690470655141E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>9000</v>
       </c>
@@ -483,8 +553,16 @@
       <c r="D5">
         <v>10500</v>
       </c>
+      <c r="E5" s="2">
+        <v>0.37445074093644898</v>
+      </c>
+      <c r="F5" s="3">
+        <f t="shared" si="0"/>
+        <v>-5.0740936448967489E-5</v>
+      </c>
+      <c r="G5" s="6"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>9500</v>
       </c>
@@ -497,8 +575,23 @@
       <c r="D6">
         <v>9781.52</v>
       </c>
+      <c r="E6" s="2">
+        <v>0.40994366040198499</v>
+      </c>
+      <c r="F6" s="3">
+        <f t="shared" si="0"/>
+        <v>32.470656339598015</v>
+      </c>
+      <c r="G6" s="7">
+        <f>(F6-$F$2)</f>
+        <v>13.050599999999807</v>
+      </c>
+      <c r="H6" s="4">
+        <f>G6/$F$2</f>
+        <v>0.67201658799460606</v>
+      </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>9500</v>
       </c>
@@ -511,6 +604,14 @@
       <c r="D7">
         <v>10500</v>
       </c>
+      <c r="E7" s="2">
+        <v>0.37703065854857298</v>
+      </c>
+      <c r="F7" s="3">
+        <f t="shared" si="0"/>
+        <v>-6.5854857300706726E-7</v>
+      </c>
+      <c r="G7" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
+100m3 from 8500 to 9000
</commit_message>
<xml_diff>
--- a/main/results/CIRED/FinalValuesCIREDResults.xlsx
+++ b/main/results/CIRED/FinalValuesCIREDResults.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergi Costa\Documents\agistin\main\results\CIRED\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07ED3C66-6481-4553-B31C-7561A5E25212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C334F4-18E3-497A-AAAE-F48DF22D3286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4740" yWindow="2520" windowWidth="19755" windowHeight="12510" xr2:uid="{868BAA8E-1AA2-4D5F-B31E-70B0642F7C3D}"/>
+    <workbookView xWindow="3990" yWindow="1980" windowWidth="19755" windowHeight="12510" xr2:uid="{868BAA8E-1AA2-4D5F-B31E-70B0642F7C3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$H$12</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -63,7 +66,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.0000"/>
-    <numFmt numFmtId="167" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -105,7 +108,7 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -426,10 +429,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95B29B87-BC7A-4D90-BE76-F4D7E2AFE4B5}">
-  <dimension ref="A1:H7"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,7 +493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>8500</v>
       </c>
@@ -506,41 +510,41 @@
         <v>0.37253296342661602</v>
       </c>
       <c r="F3" s="3">
-        <f t="shared" ref="F3:F7" si="0">C3-E3</f>
+        <f>C3-E3</f>
         <v>-3.2963426616017255E-5</v>
       </c>
       <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>9000</v>
+        <v>8600</v>
       </c>
       <c r="B4">
         <v>8</v>
       </c>
       <c r="C4">
-        <v>19.2</v>
+        <v>19.343981281717401</v>
       </c>
       <c r="D4">
         <v>9500</v>
       </c>
       <c r="E4" s="2">
-        <v>0.40994369703737998</v>
+        <v>0</v>
       </c>
       <c r="F4" s="3">
-        <f t="shared" si="0"/>
-        <v>18.790056302962618</v>
+        <f>C4-E4</f>
+        <v>19.343981281717401</v>
       </c>
       <c r="G4" s="7">
         <f>(F4-$F$2)</f>
-        <v>-0.63000003663558957</v>
+        <v>-7.6075057880807151E-2</v>
       </c>
       <c r="H4" s="4">
         <f>G4/$F$2</f>
-        <v>-3.2440690470655141E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-3.9173448598955564E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>9000</v>
       </c>
@@ -557,41 +561,41 @@
         <v>0.37445074093644898</v>
       </c>
       <c r="F5" s="3">
-        <f t="shared" si="0"/>
+        <f>C5-E5</f>
         <v>-5.0740936448967489E-5</v>
       </c>
       <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>9500</v>
+        <v>8700</v>
       </c>
       <c r="B6">
         <v>8</v>
       </c>
-      <c r="C6" s="1">
-        <v>32.880600000000001</v>
+      <c r="C6">
+        <v>19.101166695811699</v>
       </c>
       <c r="D6">
-        <v>9781.52</v>
+        <v>9500</v>
       </c>
       <c r="E6" s="2">
-        <v>0.40994366040198499</v>
+        <v>0</v>
       </c>
       <c r="F6" s="3">
-        <f t="shared" si="0"/>
-        <v>32.470656339598015</v>
+        <f>C6-E6</f>
+        <v>19.101166695811699</v>
       </c>
       <c r="G6" s="7">
         <f>(F6-$F$2)</f>
-        <v>13.050599999999807</v>
+        <v>-0.31888964378650897</v>
       </c>
       <c r="H6" s="4">
         <f>G6/$F$2</f>
-        <v>0.67201658799460606</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-1.642063432824761E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>9500</v>
       </c>
@@ -608,12 +612,167 @@
         <v>0.37703065854857298</v>
       </c>
       <c r="F7" s="3">
-        <f t="shared" si="0"/>
+        <f>C7-E7</f>
         <v>-6.5854857300706726E-7</v>
       </c>
       <c r="G7" s="6"/>
     </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8800</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>18.938235990747199</v>
+      </c>
+      <c r="D8">
+        <v>9500</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3">
+        <f>C8-E8</f>
+        <v>18.938235990747199</v>
+      </c>
+      <c r="G8" s="7">
+        <f>(F8-$F$2)</f>
+        <v>-0.48182034885100933</v>
+      </c>
+      <c r="H8" s="4">
+        <f>G8/$F$2</f>
+        <v>-2.481045061998919E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8900</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>18.856681517719199</v>
+      </c>
+      <c r="D9">
+        <v>9500</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3">
+        <f>C9-E9</f>
+        <v>18.856681517719199</v>
+      </c>
+      <c r="G9" s="7">
+        <f>(F9-$F$2)</f>
+        <v>-0.56337482187900889</v>
+      </c>
+      <c r="H9" s="4">
+        <f>G9/$F$2</f>
+        <v>-2.9009947861493426E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9000</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>19.2</v>
+      </c>
+      <c r="D10">
+        <v>9500</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.40994369703737998</v>
+      </c>
+      <c r="F10" s="3">
+        <f>C10-E10</f>
+        <v>18.790056302962618</v>
+      </c>
+      <c r="G10" s="7">
+        <f>(F10-$F$2)</f>
+        <v>-0.63000003663558957</v>
+      </c>
+      <c r="H10" s="4">
+        <f>G10/$F$2</f>
+        <v>-3.2440690470655141E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9100</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>18.7701387726127</v>
+      </c>
+      <c r="D11">
+        <v>9500</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3">
+        <f>C11-E11</f>
+        <v>18.7701387726127</v>
+      </c>
+      <c r="G11" s="7">
+        <f>(F11-$F$2)</f>
+        <v>-0.64991756698550773</v>
+      </c>
+      <c r="H11" s="4">
+        <f>G11/$F$2</f>
+        <v>-3.3466306977714681E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>9500</v>
+      </c>
+      <c r="B12">
+        <v>8</v>
+      </c>
+      <c r="C12" s="1">
+        <v>32.880600000000001</v>
+      </c>
+      <c r="D12">
+        <v>9781.52</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.40994366040198499</v>
+      </c>
+      <c r="F12" s="3">
+        <f>C12-E12</f>
+        <v>32.470656339598015</v>
+      </c>
+      <c r="G12" s="7">
+        <f>(F12-$F$2)</f>
+        <v>13.050599999999807</v>
+      </c>
+      <c r="H12" s="4">
+        <f>G12/$F$2</f>
+        <v>0.67201658799460606</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:H12" xr:uid="{95B29B87-BC7A-4D90-BE76-F4D7E2AFE4B5}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="8"/>
+      </filters>
+    </filterColumn>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H12">
+      <sortCondition ref="A1:A12"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>